<commit_message>
fix: more environments added
</commit_message>
<xml_diff>
--- a/descriptions.xlsx
+++ b/descriptions.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="45">
   <si>
     <t>skills</t>
   </si>
@@ -116,6 +116,42 @@
   </si>
   <si>
     <t>Скрита пътека</t>
+  </si>
+  <si>
+    <t>+2 скорост</t>
+  </si>
+  <si>
+    <t>Тайна пътека</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Магическо влияние</t>
+  </si>
+  <si>
+    <t>-3 живот</t>
+  </si>
+  <si>
+    <t>Номер</t>
+  </si>
+  <si>
+    <t>-2 скорост</t>
+  </si>
+  <si>
+    <t>Бодливи храсти</t>
+  </si>
+  <si>
+    <t>Суша</t>
+  </si>
+  <si>
+    <t>-1 живот, +1 скорост</t>
+  </si>
+  <si>
+    <t>Буря</t>
+  </si>
+  <si>
+    <t>Дъжд</t>
   </si>
 </sst>
 </file>
@@ -724,383 +760,716 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="48.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="48.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>32</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
       <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
       <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
       <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
       <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
       <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
       <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
         <v>21</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
       <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
       <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
       <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
       <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
       <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
       <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
       <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
       <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
       <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
       <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
       <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
       <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
       <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="D30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
         <v>25</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
       <c r="B32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
       <c r="B33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+      <c r="D33" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="C34" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="C35" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="C36" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>35</v>
+      </c>
       <c r="B37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="D37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
         <v>23</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="D38" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
         <v>24</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="D39" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>30</v>
+      </c>
+      <c r="C43" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>27</v>
-      </c>
-      <c r="B40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C40" s="4" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>30</v>
-      </c>
-      <c r="B41" t="s">
-        <v>17</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>30</v>
-      </c>
-      <c r="B42" t="s">
-        <v>17</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>30</v>
-      </c>
-      <c r="B43" t="s">
-        <v>17</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>29</v>
-      </c>
-      <c r="B45" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="C47" t="s">
         <v>18</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="C48" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="C49" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="C50" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>35</v>
+      </c>
+      <c r="C51" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>50</v>
+      </c>
       <c r="B52" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+      <c r="D52" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="C53" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="C54" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="C55" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="C56" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="C57" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>56</v>
+      </c>
       <c r="B58" t="s">
+        <v>35</v>
+      </c>
+      <c r="C58" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: some environments and zones added
</commit_message>
<xml_diff>
--- a/descriptions.xlsx
+++ b/descriptions.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="45">
   <si>
     <t>skills</t>
   </si>
@@ -760,10 +760,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,9 +796,6 @@
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
       <c r="B3" t="s">
         <v>21</v>
       </c>
@@ -810,9 +807,6 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
@@ -824,647 +818,746 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" t="s">
-        <v>35</v>
+      <c r="D9" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
+      <c r="B10" t="s">
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
+      <c r="B11" t="s">
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10</v>
+      <c r="B12" t="s">
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>11</v>
-      </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>12</v>
-      </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>13</v>
-      </c>
       <c r="C15" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>35</v>
-      </c>
       <c r="C16" t="s">
         <v>14</v>
       </c>
-      <c r="D16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>21</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>35</v>
       </c>
       <c r="C23" t="s">
         <v>20</v>
       </c>
-      <c r="D23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="D23" s="4" t="s">
         <v>22</v>
       </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>23</v>
-      </c>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>24</v>
-      </c>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>25</v>
-      </c>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>26</v>
-      </c>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>27</v>
-      </c>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>28</v>
-      </c>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" t="s">
         <v>15</v>
-      </c>
-      <c r="D30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" t="s">
-        <v>16</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>32</v>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>24</v>
       </c>
       <c r="C34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="D43" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>36</v>
+      </c>
+      <c r="C47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C35" t="s">
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>30</v>
+      </c>
+      <c r="C49" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>34</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="D49" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>30</v>
+      </c>
+      <c r="C50" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>35</v>
-      </c>
-      <c r="B37" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="D50" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>35</v>
+      </c>
+      <c r="C51" t="s">
         <v>16</v>
       </c>
-      <c r="D37" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>36</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="D51" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" t="s">
+        <v>16</v>
+      </c>
+      <c r="D52" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
         <v>23</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C53" t="s">
         <v>17</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D53" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>37</v>
-      </c>
-      <c r="B39" t="s">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
         <v>24</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C55" t="s">
         <v>17</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D55" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>38</v>
-      </c>
-      <c r="B40" t="s">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
         <v>27</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C56" t="s">
         <v>17</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D56" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>30</v>
+      </c>
+      <c r="C57" t="s">
+        <v>17</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>30</v>
+      </c>
+      <c r="C58" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>30</v>
+      </c>
+      <c r="C59" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>30</v>
+      </c>
+      <c r="C60" t="s">
+        <v>17</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>35</v>
+      </c>
+      <c r="C61" t="s">
+        <v>17</v>
+      </c>
+      <c r="D61" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>35</v>
+      </c>
+      <c r="C62" t="s">
+        <v>17</v>
+      </c>
+      <c r="D62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>29</v>
+      </c>
+      <c r="C63" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B41" t="s">
-        <v>30</v>
-      </c>
-      <c r="C41" t="s">
-        <v>17</v>
-      </c>
-      <c r="D41" s="4" t="s">
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>29</v>
+      </c>
+      <c r="C64" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>21</v>
+      </c>
+      <c r="C65" t="s">
+        <v>18</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>21</v>
+      </c>
+      <c r="C66" t="s">
+        <v>18</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>41</v>
+      </c>
+      <c r="C67" t="s">
+        <v>18</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>41</v>
+      </c>
+      <c r="C68" t="s">
+        <v>18</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>30</v>
+      </c>
+      <c r="C69" t="s">
+        <v>18</v>
+      </c>
+      <c r="D69" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>40</v>
-      </c>
-      <c r="B42" t="s">
-        <v>30</v>
-      </c>
-      <c r="C42" t="s">
-        <v>17</v>
-      </c>
-      <c r="D42" s="4" t="s">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>30</v>
+      </c>
+      <c r="C70" t="s">
+        <v>18</v>
+      </c>
+      <c r="D70" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>41</v>
-      </c>
-      <c r="B43" t="s">
-        <v>30</v>
-      </c>
-      <c r="C43" t="s">
-        <v>17</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>42</v>
-      </c>
-      <c r="B44" t="s">
-        <v>35</v>
-      </c>
-      <c r="C44" t="s">
-        <v>17</v>
-      </c>
-      <c r="D44" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>43</v>
-      </c>
-      <c r="B45" t="s">
-        <v>29</v>
-      </c>
-      <c r="C45" t="s">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>35</v>
+      </c>
+      <c r="C71" t="s">
         <v>18</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>44</v>
-      </c>
-      <c r="B46" t="s">
-        <v>21</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="D71" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>35</v>
+      </c>
+      <c r="C72" t="s">
         <v>18</v>
       </c>
-      <c r="D46" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>45</v>
-      </c>
-      <c r="C47" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>46</v>
-      </c>
-      <c r="C48" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>47</v>
-      </c>
-      <c r="C49" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>48</v>
-      </c>
-      <c r="C50" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>49</v>
-      </c>
-      <c r="B51" t="s">
-        <v>35</v>
-      </c>
-      <c r="C51" t="s">
-        <v>18</v>
-      </c>
-      <c r="D51" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>50</v>
-      </c>
-      <c r="B52" t="s">
+      <c r="D72" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
         <v>25</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C73" t="s">
         <v>19</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D73" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>51</v>
-      </c>
-      <c r="C53" t="s">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>52</v>
-      </c>
-      <c r="C54" t="s">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>53</v>
-      </c>
-      <c r="C55" t="s">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>54</v>
-      </c>
-      <c r="C56" t="s">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>55</v>
-      </c>
-      <c r="C57" t="s">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>56</v>
-      </c>
-      <c r="B58" t="s">
-        <v>35</v>
-      </c>
-      <c r="C58" t="s">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>35</v>
+      </c>
+      <c r="C79" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: some descriptions added
</commit_message>
<xml_diff>
--- a/descriptions.xlsx
+++ b/descriptions.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="14220" windowHeight="8325" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="14220" windowHeight="8325" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SUMMARY" sheetId="2" r:id="rId1"/>
-    <sheet name="skills" sheetId="1" r:id="rId2"/>
-    <sheet name="zone types" sheetId="4" r:id="rId3"/>
-    <sheet name="environments" sheetId="3" r:id="rId4"/>
+    <sheet name="classes" sheetId="5" r:id="rId2"/>
+    <sheet name="skills" sheetId="1" r:id="rId3"/>
+    <sheet name="zone types" sheetId="4" r:id="rId4"/>
+    <sheet name="environments" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="59">
   <si>
     <t>skills</t>
   </si>
@@ -152,13 +153,55 @@
   </si>
   <si>
     <t>Дъжд</t>
+  </si>
+  <si>
+    <t>Роля</t>
+  </si>
+  <si>
+    <t>Джудже боец</t>
+  </si>
+  <si>
+    <t>танк</t>
+  </si>
+  <si>
+    <t>Полуръст разбойник</t>
+  </si>
+  <si>
+    <t>меле DD</t>
+  </si>
+  <si>
+    <t>Човек магьосник</t>
+  </si>
+  <si>
+    <t>range DD</t>
+  </si>
+  <si>
+    <t>Елф рейнджър</t>
+  </si>
+  <si>
+    <t>Човек вещица</t>
+  </si>
+  <si>
+    <t>лечител</t>
+  </si>
+  <si>
+    <t>Джудже паладин</t>
+  </si>
+  <si>
+    <t>Елф свещеник</t>
+  </si>
+  <si>
+    <t>Човек паладин</t>
+  </si>
+  <si>
+    <t>Раса и клас</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,8 +220,26 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,8 +252,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -200,16 +267,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,6 +768,253 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="15" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11"/>
+    </row>
+    <row r="2" spans="1:16" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+    </row>
+    <row r="3" spans="1:16" ht="1.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="11"/>
+    </row>
+    <row r="4" spans="1:16" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13"/>
+      <c r="B4" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+    </row>
+    <row r="5" spans="1:16" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="13"/>
+      <c r="B5" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+    </row>
+    <row r="6" spans="1:16" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+    </row>
+    <row r="7" spans="1:16" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="13"/>
+      <c r="B7" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+    </row>
+    <row r="8" spans="1:16" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="13"/>
+      <c r="B8" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+    </row>
+    <row r="9" spans="1:16" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="13"/>
+      <c r="B9" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+    </row>
+    <row r="10" spans="1:16" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
+      <c r="B10" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+    </row>
+    <row r="11" spans="1:16" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
+      <c r="B11" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -697,59 +1059,64 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A10"/>
+  <dimension ref="B2:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="2" spans="2:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" ht="1.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="7"/>
+    </row>
+    <row r="4" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B4" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B5" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B6" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B7" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B8" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B9" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B10" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B11" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -758,11 +1125,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix: quest zones list added, village zones list added
</commit_message>
<xml_diff>
--- a/descriptions.xlsx
+++ b/descriptions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="14220" windowHeight="8325" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="14220" windowHeight="8325" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="SUMMARY" sheetId="2" r:id="rId1"/>
@@ -12,13 +12,15 @@
     <sheet name="skills" sheetId="1" r:id="rId3"/>
     <sheet name="zone types" sheetId="4" r:id="rId4"/>
     <sheet name="environments" sheetId="3" r:id="rId5"/>
+    <sheet name="quest zones list" sheetId="6" r:id="rId6"/>
+    <sheet name="village zones list" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="94">
   <si>
     <t>skills</t>
   </si>
@@ -195,6 +197,865 @@
   </si>
   <si>
     <t>Раса и клас</t>
+  </si>
+  <si>
+    <t>classes</t>
+  </si>
+  <si>
+    <t>quest zones list</t>
+  </si>
+  <si>
+    <t>Фонтан на младостта</t>
+  </si>
+  <si>
+    <t>Олтар на душите</t>
+  </si>
+  <si>
+    <t>Кула на магьосника</t>
+  </si>
+  <si>
+    <t>Прокълнат манастир</t>
+  </si>
+  <si>
+    <t>Гнилото мочурище</t>
+  </si>
+  <si>
+    <t>Изоставена златна мина</t>
+  </si>
+  <si>
+    <t>Забравеното село</t>
+  </si>
+  <si>
+    <t>Кралска крепост</t>
+  </si>
+  <si>
+    <t>Призрачен град</t>
+  </si>
+  <si>
+    <t>Криптата</t>
+  </si>
+  <si>
+    <t>Червена пустош</t>
+  </si>
+  <si>
+    <t>Ледената тундра</t>
+  </si>
+  <si>
+    <t>Гъстата дъбрава</t>
+  </si>
+  <si>
+    <t>Брулени хълмове</t>
+  </si>
+  <si>
+    <t>quests</t>
+  </si>
+  <si>
+    <t>93 x 59 mm</t>
+  </si>
+  <si>
+    <t>Цена</t>
+  </si>
+  <si>
+    <t>1 време</t>
+  </si>
+  <si>
+    <t>Ковачница</t>
+  </si>
+  <si>
+    <t>Магьосническо ателие</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Разкрийте следващият </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ВЪЛШЕБЕН ПРЕДМЕТ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Можете да го закупите на посочената цена (трябва да имате или да осигурите поне едно свободно място в </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>РАНИЦАТА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> или </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ТОРБАТА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> си). Ако го закупите, приберете </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ВЪЛШЕБНИЯ ПРЕДМЕТ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">в свободно място в раницата или торбата Ви. След това сложете токен за </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>НЕДОСТЪПНОСТ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> на тестето с </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ВЪЛШЕБНИ ПРЕДМЕТИ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+2. Можете да продадете неограничено количество от </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>РЕЛИКВИТЕ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> в екипировката Ви и </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ВЪЛШЕБНИТЕ ПРЕДМЕТИ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> в инвентара Ви, които имат посочена </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ЦЕНА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> на стойност половината от посочената им </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ЦЕНА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+3. Горните две действия можете да изпълните в произволен ред (пример: теглите </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ВЪЛШЕБЕН ПРЕДМЕТ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, продавате притежавани от Вас </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>РЕЛИКВИ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> и </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ВЪЛШЕБНИ ПРЕДМЕТИ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, след това купувате изтегления </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ВЪЛШЕБЕН ПРЕДМЕТ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">).
+4. След като приключите, сложете токен за </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>НЕДОСТЪПНОСТ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> на магьосническото ателие докато не излезнете от града (ако не закупите изтегления </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ВЪЛШЕБЕН ПРЕДМЕТ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, изхвърлете картата).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Разкрийте следващата </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>РЕЛИКВА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Можете да я закупите на посочената цена. Ако я закупите, вземете токена съответстващ на </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>РЕЛИКВАТА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> и организирайте </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ЕКИПИРОВКАТА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> си. След това изхвърлете картата и сложете токен за </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">НЕДОСТЪПНОСТ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">на тестето с </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>РЕЛИКВИ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+2. Можете да продадете неограничено количество от </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>РЕЛИКВИТЕ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> в екипировката Ви и </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ВЪЛШЕБНИТЕ ПРЕДМЕТИ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> в инвентара Ви, които имат посочена </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ЦЕНА </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">на стойност половината от посочената им </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ЦЕНА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+3. Горните две действия можете да изпълните в произволен ред (пример: теглите </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>РЕЛИКВА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, продавате притежавани от Вас </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>РЕЛИКВИ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> и </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ВЪЛШЕБНИ ПРЕДМЕТИ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, след това купувате изтеглената </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>РЕЛИКВА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">).
+4. След като приключите, сложете токен за </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">НЕДОСТЪПНОСТ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">на ковачницата докато не излезнете от града (ако не закупите изтеглената </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>РЕЛИКВА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, изхвърлете картата).</t>
+    </r>
+  </si>
+  <si>
+    <t>Алхимическа лаборатория</t>
+  </si>
+  <si>
+    <t>Страноприемница</t>
+  </si>
+  <si>
+    <t>Кметство</t>
+  </si>
+  <si>
+    <t>Църква</t>
+  </si>
+  <si>
+    <t>Гилдия на гадателите</t>
+  </si>
+  <si>
+    <t>0 време</t>
+  </si>
+  <si>
+    <t>лековити отвари</t>
+  </si>
+  <si>
+    <t>храна, почивка</t>
+  </si>
+  <si>
+    <t>странични мисии</t>
+  </si>
+  <si>
+    <t>анкхове</t>
+  </si>
+  <si>
+    <t>градски събития</t>
   </si>
 </sst>
 </file>
@@ -299,7 +1160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -325,6 +1186,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,7 +1494,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,16 +1523,17 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
+      <c r="B3" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="19"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -675,25 +1541,37 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1063,7 +1941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -1934,4 +2812,239 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:A16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="71.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" ht="240" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="20"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="20"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" s="20"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" s="20"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" s="20"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" s="20"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" s="20"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="20"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="20"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="20"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix: some quests added
</commit_message>
<xml_diff>
--- a/descriptions.xlsx
+++ b/descriptions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="14220" windowHeight="8325" activeTab="6"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="14220" windowHeight="8325" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="SUMMARY" sheetId="2" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="environments" sheetId="3" r:id="rId5"/>
     <sheet name="quest zones list" sheetId="6" r:id="rId6"/>
     <sheet name="village zones list" sheetId="7" r:id="rId7"/>
+    <sheet name="quests" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="118">
   <si>
     <t>skills</t>
   </si>
@@ -265,8 +266,50 @@
     <t>Магьосническо ателие</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. Разкрийте следващият </t>
+    <t>Алхимическа лаборатория</t>
+  </si>
+  <si>
+    <t>Страноприемница</t>
+  </si>
+  <si>
+    <t>Кметство</t>
+  </si>
+  <si>
+    <t>Църква</t>
+  </si>
+  <si>
+    <t>Гилдия на гадателите</t>
+  </si>
+  <si>
+    <t>0 време</t>
+  </si>
+  <si>
+    <t>лековити отвари</t>
+  </si>
+  <si>
+    <t>храна, почивка</t>
+  </si>
+  <si>
+    <t>странични мисии</t>
+  </si>
+  <si>
+    <t>анкхове</t>
+  </si>
+  <si>
+    <t>градски събития</t>
+  </si>
+  <si>
+    <t>Действие</t>
+  </si>
+  <si>
+    <t>Набитото брадато джудже изглежда страховито в тежката броня, но е весело и ухилено. Замисляш се дали си заслужава да провериш върху какво работи. А може би е по-добре да се отървеш от няколко безполезни вехтории в раницата си.</t>
+  </si>
+  <si>
+    <t>Островърхата шапка на елфа само подчертава типичната за магьосниците надменност, но въпреки това се оказва услужлив и ти показва стоката си.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Разкрий следващата </t>
     </r>
     <r>
       <rPr>
@@ -279,18 +322,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ВЪЛШЕБЕН ПРЕДМЕТ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. Можете да го закупите на посочената цена (трябва да имате или да осигурите поне едно свободно място в </t>
+      <t>РЕЛИКВА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Можеш да я закупиш на посочената цена. Ако я закупиш, вземи токена съответстващ на </t>
     </r>
     <r>
       <rPr>
@@ -303,18 +346,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>РАНИЦАТА</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> или </t>
+      <t>РЕЛИКВАТА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> и организирай </t>
     </r>
     <r>
       <rPr>
@@ -327,18 +370,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ТОРБАТА</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> си). Ако го закупите, приберете </t>
+      <t>ЕКИПИРОВКАТА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> си. След това изхвърли картата и сложи токен за </t>
     </r>
     <r>
       <rPr>
@@ -351,18 +394,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">ВЪЛШЕБНИЯ ПРЕДМЕТ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">в свободно място в раницата или торбата Ви. След това сложете токен за </t>
+      <t xml:space="preserve">НЕДОСТЪПНОСТ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">на тестето с </t>
     </r>
     <r>
       <rPr>
@@ -375,18 +418,19 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>НЕДОСТЪПНОСТ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> на тестето с </t>
+      <t>РЕЛИКВИ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+2. Можеш да продадеш неограничено количество от </t>
     </r>
     <r>
       <rPr>
@@ -399,19 +443,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ВЪЛШЕБНИ ПРЕДМЕТИ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.
-2. Можете да продадете неограничено количество от </t>
+      <t>РЕЛИКВИТЕ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> в екипировката си и </t>
     </r>
     <r>
       <rPr>
@@ -424,18 +467,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>РЕЛИКВИТЕ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> в екипировката Ви и </t>
+      <t>ВЪЛШЕБНИТЕ ПРЕДМЕТИ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> в инвентара си, които имат посочена </t>
     </r>
     <r>
       <rPr>
@@ -448,18 +491,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ВЪЛШЕБНИТЕ ПРЕДМЕТИ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> в инвентара Ви, които имат посочена </t>
+      <t xml:space="preserve">ЦЕНА </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">на стойност половината от посочената им </t>
     </r>
     <r>
       <rPr>
@@ -483,7 +526,8 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> на стойност половината от посочената им </t>
+      <t xml:space="preserve">.
+3. Горните две действия можеш да изпълниш в произволен ред (пример: теглиш </t>
     </r>
     <r>
       <rPr>
@@ -496,19 +540,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ЦЕНА</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.
-3. Горните две действия можете да изпълните в произволен ред (пример: теглите </t>
+      <t>РЕЛИКВА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, продаваш притежавани от теб </t>
     </r>
     <r>
       <rPr>
@@ -521,18 +564,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ВЪЛШЕБЕН ПРЕДМЕТ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, продавате притежавани от Вас </t>
+      <t>РЕЛИКВИ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> и </t>
     </r>
     <r>
       <rPr>
@@ -545,18 +588,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>РЕЛИКВИ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> и </t>
+      <t>ВЪЛШЕБНИ ПРЕДМЕТИ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, след това купуваш изтеглената </t>
     </r>
     <r>
       <rPr>
@@ -569,18 +612,19 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ВЪЛШЕБНИ ПРЕДМЕТИ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, след това купувате изтегления </t>
+      <t>РЕЛИКВА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">).
+4. След като приключиш, сложи токен за </t>
     </r>
     <r>
       <rPr>
@@ -593,19 +637,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ВЪЛШЕБЕН ПРЕДМЕТ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">).
-4. След като приключите, сложете токен за </t>
+      <t xml:space="preserve">НЕДОСТЪПНОСТ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">на ковачницата докато не излезнеш от града (ако не закупиш изтеглената </t>
     </r>
     <r>
       <rPr>
@@ -618,18 +661,23 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>НЕДОСТЪПНОСТ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> на магьосническото ателие докато не излезнете от града (ако не закупите изтегления </t>
+      <t>РЕЛИКВА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, изхвърли картата).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Разкрий следващите два </t>
     </r>
     <r>
       <rPr>
@@ -642,23 +690,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ВЪЛШЕБЕН ПРЕДМЕТ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, изхвърлете картата).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. Разкрийте следващата </t>
+      <t>ВЪЛШЕБНИ ПРЕДМЕТА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. След това сложи токен за </t>
     </r>
     <r>
       <rPr>
@@ -671,18 +714,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>РЕЛИКВА</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. Можете да я закупите на посочената цена. Ако я закупите, вземете токена съответстващ на </t>
+      <t>НЕДОСТЪПНОСТ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> на тестето с </t>
     </r>
     <r>
       <rPr>
@@ -695,18 +738,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>РЕЛИКВАТА</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> и организирайте </t>
+      <t>ВЪЛШЕБНИ ПРЕДМЕТИ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Можеш да закупиш всеки от тях на посочената цена (трябва да имаш или да осигуриш поне едно свободно място в </t>
     </r>
     <r>
       <rPr>
@@ -719,18 +762,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ЕКИПИРОВКАТА</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> си. След това изхвърлете картата и сложете токен за </t>
+      <t>РАНИЦАТА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> или </t>
     </r>
     <r>
       <rPr>
@@ -743,18 +786,19 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">НЕДОСТЪПНОСТ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">на тестето с </t>
+      <t>ТОРБАТА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> си за всеки, който закупиш). Ако закупиш който и да е, приберш го в свободно място в раницата или торбата си.
+2. Можеш да продадеш неограничено количество от </t>
     </r>
     <r>
       <rPr>
@@ -767,19 +811,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>РЕЛИКВИ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.
-2. Можете да продадете неограничено количество от </t>
+      <t>РЕЛИКВИТЕ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> в екипировката си и </t>
     </r>
     <r>
       <rPr>
@@ -792,18 +835,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>РЕЛИКВИТЕ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> в екипировката Ви и </t>
+      <t>ВЪЛШЕБНИТЕ ПРЕДМЕТИ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> в инвентара си, които имат посочена </t>
     </r>
     <r>
       <rPr>
@@ -816,18 +859,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ВЪЛШЕБНИТЕ ПРЕДМЕТИ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> в инвентара Ви, които имат посочена </t>
+      <t>ЦЕНА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> на стойност половината от посочената им </t>
     </r>
     <r>
       <rPr>
@@ -840,18 +883,19 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">ЦЕНА </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">на стойност половината от посочената им </t>
+      <t>ЦЕНА</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+3. Горните две действия можеш да изпълниш в произволен ред (пример: теглиш </t>
     </r>
     <r>
       <rPr>
@@ -864,19 +908,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ЦЕНА</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.
-3. Горните две действия можете да изпълните в произволен ред (пример: теглите </t>
+      <t>ВЪЛШЕБНИ ПРЕДМЕТИ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, продаваш притежавани от теб </t>
     </r>
     <r>
       <rPr>
@@ -889,18 +932,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>РЕЛИКВА</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, продавате притежавани от Вас </t>
+      <t>РЕЛИКВИ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> и </t>
     </r>
     <r>
       <rPr>
@@ -913,18 +956,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>РЕЛИКВИ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> и </t>
+      <t>ВЪЛШЕБНИ ПРЕДМЕТИ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, след това купуваш изтеглен </t>
     </r>
     <r>
       <rPr>
@@ -937,18 +980,19 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ВЪЛШЕБНИ ПРЕДМЕТИ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, след това купувате изтеглената </t>
+      <t>ВЪЛШЕБЕН ПРЕДМЕТ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">).
+4. След като приключиш, изхвърли картата на всеки незакупен </t>
     </r>
     <r>
       <rPr>
@@ -961,19 +1005,18 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>РЕЛИКВА</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">).
-4. След като приключите, сложете токен за </t>
+      <t>ВЪЛШЕБЕН ПРЕДМЕТ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Сложи токен за </t>
     </r>
     <r>
       <rPr>
@@ -986,76 +1029,82 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">НЕДОСТЪПНОСТ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">на ковачницата докато не излезнете от града (ако не закупите изтеглената </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>РЕЛИКВА</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, изхвърлете картата).</t>
-    </r>
-  </si>
-  <si>
-    <t>Алхимическа лаборатория</t>
-  </si>
-  <si>
-    <t>Страноприемница</t>
-  </si>
-  <si>
-    <t>Кметство</t>
-  </si>
-  <si>
-    <t>Църква</t>
-  </si>
-  <si>
-    <t>Гилдия на гадателите</t>
-  </si>
-  <si>
-    <t>0 време</t>
-  </si>
-  <si>
-    <t>лековити отвари</t>
-  </si>
-  <si>
-    <t>храна, почивка</t>
-  </si>
-  <si>
-    <t>странични мисии</t>
-  </si>
-  <si>
-    <t>анкхове</t>
-  </si>
-  <si>
-    <t>градски събития</t>
+      <t>НЕДОСТЪПНОСТ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> на магьосническото ателие докато не излезнеш от града.</t>
+    </r>
+  </si>
+  <si>
+    <t>Група гноми се щурат като мравки между бълбукащите стъкленици и колби. Един гном с дебели ръкавици стои пред рафт с готови субстанции. Може би някои от тези шишенца биха се оказали полезни.</t>
+  </si>
+  <si>
+    <t>Въпреки, че са силно обвързани с религията си, монасите се оказват готови на добра сделка.</t>
+  </si>
+  <si>
+    <t>Зона</t>
+  </si>
+  <si>
+    <t>Трудност</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Изгубеният остров</t>
+  </si>
+  <si>
+    <t>Островът, на който се намира Фонтана на младостта е изчезнал. Носят се слухове, че е преместен с помощта на магия от зъл магьосник, водещ армия слуги.</t>
+  </si>
+  <si>
+    <t>Цел</t>
+  </si>
+  <si>
+    <t>Начален епизод</t>
+  </si>
+  <si>
+    <t>***</t>
+  </si>
+  <si>
+    <t>Открий магьосника и разбери местоположението на изгубения остров.</t>
+  </si>
+  <si>
+    <t>Пиратско нашествие</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>Морско чудовище</t>
+  </si>
+  <si>
+    <t>Островът с Фонтанът на младостта е превзет от огромно морско чудовище и никой няма достъп до фонтана.</t>
+  </si>
+  <si>
+    <t>Островът с Фонтана на младостта е превзет от пирати, които продават благата му на огромна цена.</t>
+  </si>
+  <si>
+    <t>Спасение за краля</t>
+  </si>
+  <si>
+    <t>Местния владетел е смъртно ранен. Синовете му биха дали всичко, за да го спасят.</t>
+  </si>
+  <si>
+    <t>Прогони чудовището, охраняващо острова.</t>
+  </si>
+  <si>
+    <t>Прогони пиратите от острова.</t>
+  </si>
+  <si>
+    <t>Донеси колба с вода от Фонтана на младостта.</t>
   </si>
 </sst>
 </file>
@@ -1160,7 +1209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1188,6 +1237,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2819,7 +2871,7 @@
   <dimension ref="A3:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A3" sqref="A3:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2904,20 +2956,21 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.140625" customWidth="1"/>
     <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.7109375" customWidth="1"/>
+    <col min="4" max="4" width="71.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2927,13 +2980,17 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" ht="240" x14ac:dyDescent="0.25">
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" ht="240" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>80</v>
       </c>
@@ -2941,10 +2998,13 @@
         <v>78</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -2952,96 +3012,556 @@
         <v>78</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
         <v>78</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B6" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="20" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="20"/>
+      <c r="D6" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
         <v>78</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" s="20"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="20"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" s="20"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="20"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" s="20"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="20"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C13" s="20"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="20"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" s="20"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="20"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" s="20"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="20"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" s="20"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="20"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="20"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="20"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="20"/>
+      <c r="D16" s="20"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="20"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="20"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="20"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+    </row>
+    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+    </row>
+    <row r="25" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+    </row>
+    <row r="26" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+    </row>
+    <row r="27" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+    </row>
+    <row r="28" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+    </row>
+    <row r="29" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+    </row>
+    <row r="30" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+    </row>
+    <row r="31" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+    </row>
+    <row r="32" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+    </row>
+    <row r="38" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>68</v>
+      </c>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+    </row>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>70</v>
+      </c>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+    </row>
+    <row r="41" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>71</v>
+      </c>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+    </row>
+    <row r="42" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>72</v>
+      </c>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+    </row>
+    <row r="43" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>73</v>
+      </c>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+    </row>
+    <row r="44" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>74</v>
+      </c>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+    </row>
+    <row r="45" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+    </row>
+    <row r="46" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+    </row>
+    <row r="47" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+    </row>
+    <row r="48" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+    </row>
+    <row r="49" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+    </row>
+    <row r="50" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+    </row>
+    <row r="51" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+    </row>
+    <row r="52" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+    </row>
+    <row r="53" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+    </row>
+    <row r="54" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
+    </row>
+    <row r="55" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+    </row>
+    <row r="56" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
+    </row>
+    <row r="57" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
+    </row>
+    <row r="58" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
+    </row>
+    <row r="59" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+    </row>
+    <row r="60" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E60" s="20"/>
+      <c r="F60" s="20"/>
+    </row>
+    <row r="61" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E61" s="20"/>
+      <c r="F61" s="20"/>
+    </row>
+    <row r="62" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E62" s="20"/>
+      <c r="F62" s="20"/>
+    </row>
+    <row r="63" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E63" s="20"/>
+      <c r="F63" s="20"/>
+    </row>
+    <row r="64" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E64" s="20"/>
+      <c r="F64" s="20"/>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F65" s="20"/>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F66" s="20"/>
+    </row>
+    <row r="67" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F67" s="20"/>
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F68" s="20"/>
+    </row>
+    <row r="69" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F69" s="20"/>
+    </row>
+    <row r="70" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F70" s="20"/>
+    </row>
+    <row r="71" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F71" s="20"/>
+    </row>
+    <row r="72" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F72" s="20"/>
+    </row>
+    <row r="73" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F73" s="20"/>
+    </row>
+    <row r="74" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F74" s="20"/>
+    </row>
+    <row r="75" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F75" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>